<commit_message>
Finished writing the first version of the hamilton product in simd. Haven't benchmarked it.
Still need to finish other functions in simd quaternion class.
</commit_message>
<xml_diff>
--- a/build/Visual Studio Community 2022 Release - amd64/Debug/Debug/GLMREGComparison.xlsx
+++ b/build/Visual Studio Community 2022 Release - amd64/Debug/Debug/GLMREGComparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelson\Documents\Projects\typed_squirrel\build\Visual Studio Community 2022 Release - amd64\Debug\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630D796D-3060-4B79-AF68-CC033FB74B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9B8ACA-5747-43D9-A60A-E7CC1FC652F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1605" yWindow="2910" windowWidth="20880" windowHeight="15705" xr2:uid="{F65BA0A3-315E-4F3B-9DC6-AB09C013BE12}"/>
   </bookViews>
@@ -1093,7 +1093,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:G46"/>
+      <selection activeCell="E2" sqref="E2:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1142,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>199</v>
+        <v>195.8</v>
       </c>
       <c r="D2" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1155,7 +1155,7 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <v>174.4</v>
+        <v>168.2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="K2">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>-24.599999999999994</v>
+        <v>-27.600000000000023</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>186</v>
+        <v>194.7</v>
       </c>
       <c r="D3" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1191,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="G3">
-        <v>206.5</v>
+        <v>205.7</v>
       </c>
       <c r="H3" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="K3">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>20.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>340.2</v>
+        <v>337.7</v>
       </c>
       <c r="D4" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1227,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="G4">
-        <v>394.8</v>
+        <v>425.1</v>
       </c>
       <c r="H4" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="K4">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>54.600000000000023</v>
+        <v>87.400000000000034</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>224.5</v>
+        <v>223.6</v>
       </c>
       <c r="D5" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1263,7 +1263,7 @@
         <v>7</v>
       </c>
       <c r="G5">
-        <v>1058.9000000000001</v>
+        <v>1054.4000000000001</v>
       </c>
       <c r="H5" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="K5">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>834.40000000000009</v>
+        <v>830.80000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1286,7 +1286,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>226.5</v>
+        <v>223.7</v>
       </c>
       <c r="D6" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1299,7 +1299,7 @@
         <v>8</v>
       </c>
       <c r="G6">
-        <v>1063.5999999999999</v>
+        <v>1055</v>
       </c>
       <c r="H6" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="K6">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>837.09999999999991</v>
+        <v>831.3</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1322,7 +1322,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>595.4</v>
+        <v>597.1</v>
       </c>
       <c r="D7" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1335,7 +1335,7 @@
         <v>9</v>
       </c>
       <c r="G7">
-        <v>1210.4000000000001</v>
+        <v>1185.5</v>
       </c>
       <c r="H7" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="K7">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>615.00000000000011</v>
+        <v>588.4</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>226.1</v>
+        <v>225.9</v>
       </c>
       <c r="D8" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1371,7 +1371,7 @@
         <v>10</v>
       </c>
       <c r="G8">
-        <v>1056.0999999999999</v>
+        <v>1050.4000000000001</v>
       </c>
       <c r="H8" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="K8">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>829.99999999999989</v>
+        <v>824.50000000000011</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D9" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1407,7 +1407,7 @@
         <v>11</v>
       </c>
       <c r="G9">
-        <v>601.79999999999995</v>
+        <v>597.6</v>
       </c>
       <c r="H9" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="K9">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>106.79999999999995</v>
+        <v>104.60000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>529.29999999999995</v>
+        <v>524</v>
       </c>
       <c r="D10" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1443,7 +1443,7 @@
         <v>12</v>
       </c>
       <c r="G10">
-        <v>1418.9</v>
+        <v>1394.9</v>
       </c>
       <c r="H10" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="K10">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>889.60000000000014</v>
+        <v>870.90000000000009</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1466,7 +1466,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>527.70000000000005</v>
+        <v>527.29999999999995</v>
       </c>
       <c r="D11" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1479,7 +1479,7 @@
         <v>13</v>
       </c>
       <c r="G11">
-        <v>1412.4</v>
+        <v>1402.9</v>
       </c>
       <c r="H11" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="K11">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>884.7</v>
+        <v>875.60000000000014</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>865.4</v>
+        <v>858</v>
       </c>
       <c r="D12" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1515,7 +1515,7 @@
         <v>14</v>
       </c>
       <c r="G12">
-        <v>1724.7</v>
+        <v>1720.3</v>
       </c>
       <c r="H12" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="K12">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>859.30000000000007</v>
+        <v>862.3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1538,7 +1538,7 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>532.4</v>
+        <v>528.79999999999995</v>
       </c>
       <c r="D13" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1551,7 +1551,7 @@
         <v>15</v>
       </c>
       <c r="G13">
-        <v>587.1</v>
+        <v>581.79999999999995</v>
       </c>
       <c r="H13" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="K13">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>54.700000000000045</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1574,7 +1574,7 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>185.7</v>
+        <v>186.6</v>
       </c>
       <c r="D14" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1587,7 +1587,7 @@
         <v>16</v>
       </c>
       <c r="G14">
-        <v>713.4</v>
+        <v>699.1</v>
       </c>
       <c r="H14" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="K14">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>527.70000000000005</v>
+        <v>512.5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1610,7 +1610,7 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>302.8</v>
+        <v>310</v>
       </c>
       <c r="D15" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1623,7 +1623,7 @@
         <v>17</v>
       </c>
       <c r="G15">
-        <v>935.6</v>
+        <v>922.5</v>
       </c>
       <c r="H15" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="K15">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>632.79999999999995</v>
+        <v>612.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>173.4</v>
+        <v>171.4</v>
       </c>
       <c r="D16" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1659,7 +1659,7 @@
         <v>18</v>
       </c>
       <c r="G16">
-        <v>173.9</v>
+        <v>171.7</v>
       </c>
       <c r="H16" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="K16">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>0.5</v>
+        <v>0.29999999999998295</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1682,7 +1682,7 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>1609.4</v>
+        <v>1593.4</v>
       </c>
       <c r="D17" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1695,7 +1695,7 @@
         <v>19</v>
       </c>
       <c r="G17">
-        <v>1759.6</v>
+        <v>1742.4</v>
       </c>
       <c r="H17" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="K17">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>150.19999999999982</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1718,7 +1718,7 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>476.4</v>
+        <v>472.4</v>
       </c>
       <c r="D18" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1731,7 +1731,7 @@
         <v>20</v>
       </c>
       <c r="G18">
-        <v>592.4</v>
+        <v>585</v>
       </c>
       <c r="H18" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="K18">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>116</v>
+        <v>112.60000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1754,7 +1754,7 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>1299.9000000000001</v>
+        <v>1284.4000000000001</v>
       </c>
       <c r="D19" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1767,7 +1767,7 @@
         <v>21</v>
       </c>
       <c r="G19">
-        <v>7114.3</v>
+        <v>7024.9</v>
       </c>
       <c r="H19" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="K19">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>5814.4</v>
+        <v>5740.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1790,7 +1790,7 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>1024.2</v>
+        <v>991</v>
       </c>
       <c r="D20" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1803,7 +1803,7 @@
         <v>22</v>
       </c>
       <c r="G20">
-        <v>7181.3</v>
+        <v>7070.1</v>
       </c>
       <c r="H20" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="K20">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>6157.1</v>
+        <v>6079.1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1826,7 +1826,7 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>2364</v>
+        <v>2385.3000000000002</v>
       </c>
       <c r="D21" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1839,7 +1839,7 @@
         <v>23</v>
       </c>
       <c r="G21">
-        <v>7120.6</v>
+        <v>7020.3</v>
       </c>
       <c r="H21" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="K21">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>4756.6000000000004</v>
+        <v>4635</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1862,7 +1862,7 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>1200.3</v>
+        <v>1193</v>
       </c>
       <c r="D22" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1875,7 +1875,7 @@
         <v>24</v>
       </c>
       <c r="G22">
-        <v>2726.3</v>
+        <v>2698.8</v>
       </c>
       <c r="H22" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="K22">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>1526.0000000000002</v>
+        <v>1505.8000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1918,11 +1918,11 @@
         <v>4</v>
       </c>
       <c r="C26" s="3">
-        <v>199</v>
+        <v>195.8</v>
       </c>
       <c r="D26" s="5" t="str">
         <f>IF(C26&lt;G26,"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>3</v>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="J26">
         <f>G26-C26</f>
-        <v>0</v>
+        <v>3.1999999999999886</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1950,7 +1950,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="4">
-        <v>186</v>
+        <v>194.7</v>
       </c>
       <c r="D27" s="5" t="str">
         <f t="shared" ref="D27:D46" si="0">IF(C27&lt;G27,"TRUE","FALSE")</f>
@@ -1967,11 +1967,11 @@
       </c>
       <c r="H27" s="5" t="str">
         <f t="shared" ref="H27:H46" si="1">IF(G27&lt;C27,"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J27">
         <f t="shared" ref="J27:J46" si="2">G27-C27</f>
-        <v>0</v>
+        <v>-8.6999999999999886</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1982,11 +1982,11 @@
         <v>6</v>
       </c>
       <c r="C28" s="3">
-        <v>340.2</v>
+        <v>337.7</v>
       </c>
       <c r="D28" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>3</v>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="J28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2014,11 +2014,11 @@
         <v>7</v>
       </c>
       <c r="C29" s="4">
-        <v>224.5</v>
+        <v>223.6</v>
       </c>
       <c r="D29" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>3</v>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="J29">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.90000000000000568</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2046,11 +2046,11 @@
         <v>8</v>
       </c>
       <c r="C30" s="3">
-        <v>226.5</v>
+        <v>223.7</v>
       </c>
       <c r="D30" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>3</v>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="J30">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.8000000000000114</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2078,7 +2078,7 @@
         <v>9</v>
       </c>
       <c r="C31" s="4">
-        <v>595.4</v>
+        <v>597.1</v>
       </c>
       <c r="D31" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2095,11 +2095,11 @@
       </c>
       <c r="H31" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1.7000000000000455</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2110,11 +2110,11 @@
         <v>10</v>
       </c>
       <c r="C32" s="3">
-        <v>226.1</v>
+        <v>225.9</v>
       </c>
       <c r="D32" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>3</v>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="J32">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.19999999999998863</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2142,11 +2142,11 @@
         <v>11</v>
       </c>
       <c r="C33" s="4">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D33" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>3</v>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="J33">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2174,11 +2174,11 @@
         <v>12</v>
       </c>
       <c r="C34" s="3">
-        <v>529.29999999999995</v>
+        <v>524</v>
       </c>
       <c r="D34" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>3</v>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="J34">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.2999999999999545</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2206,11 +2206,11 @@
         <v>13</v>
       </c>
       <c r="C35" s="4">
-        <v>527.70000000000005</v>
+        <v>527.29999999999995</v>
       </c>
       <c r="D35" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>3</v>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="J35">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.40000000000009095</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2238,11 +2238,11 @@
         <v>14</v>
       </c>
       <c r="C36" s="3">
-        <v>865.4</v>
+        <v>858</v>
       </c>
       <c r="D36" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>3</v>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="J36">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.3999999999999773</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2270,11 +2270,11 @@
         <v>15</v>
       </c>
       <c r="C37" s="4">
-        <v>532.4</v>
+        <v>528.79999999999995</v>
       </c>
       <c r="D37" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>3</v>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="J37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.6000000000000227</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2302,7 +2302,7 @@
         <v>16</v>
       </c>
       <c r="C38" s="3">
-        <v>185.7</v>
+        <v>186.6</v>
       </c>
       <c r="D38" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2319,11 +2319,11 @@
       </c>
       <c r="H38" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J38">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.90000000000000568</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
         <v>17</v>
       </c>
       <c r="C39" s="4">
-        <v>302.8</v>
+        <v>310</v>
       </c>
       <c r="D39" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2351,11 +2351,11 @@
       </c>
       <c r="H39" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-7.1999999999999886</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2366,11 +2366,11 @@
         <v>18</v>
       </c>
       <c r="C40" s="3">
-        <v>173.4</v>
+        <v>171.4</v>
       </c>
       <c r="D40" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>3</v>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="J40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2398,11 +2398,11 @@
         <v>19</v>
       </c>
       <c r="C41" s="4">
-        <v>1609.4</v>
+        <v>1593.4</v>
       </c>
       <c r="D41" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>3</v>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="J41">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2430,11 +2430,11 @@
         <v>20</v>
       </c>
       <c r="C42" s="3">
-        <v>476.4</v>
+        <v>472.4</v>
       </c>
       <c r="D42" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>3</v>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="J42">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2462,11 +2462,11 @@
         <v>21</v>
       </c>
       <c r="C43" s="4">
-        <v>1299.9000000000001</v>
+        <v>1284.4000000000001</v>
       </c>
       <c r="D43" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>3</v>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="J43">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2494,11 +2494,11 @@
         <v>22</v>
       </c>
       <c r="C44" s="3">
-        <v>1024.2</v>
+        <v>991</v>
       </c>
       <c r="D44" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>3</v>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="J44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>33.200000000000045</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
         <v>23</v>
       </c>
       <c r="C45" s="4">
-        <v>2364</v>
+        <v>2385.3000000000002</v>
       </c>
       <c r="D45" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2543,11 +2543,11 @@
       </c>
       <c r="H45" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-21.300000000000182</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2558,11 +2558,11 @@
         <v>24</v>
       </c>
       <c r="C46" s="2">
-        <v>1200.3</v>
+        <v>1193</v>
       </c>
       <c r="D46" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>3</v>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="J46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.2999999999999545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished up adding simd to most of the quaternion functions. Concluded that non-simd implementation is currently much faster and I will be shelving the simd implementation going forward.
</commit_message>
<xml_diff>
--- a/build/Visual Studio Community 2022 Release - amd64/Debug/Debug/GLMREGComparison.xlsx
+++ b/build/Visual Studio Community 2022 Release - amd64/Debug/Debug/GLMREGComparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelson\Documents\Projects\typed_squirrel\build\Visual Studio Community 2022 Release - amd64\Debug\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9B8ACA-5747-43D9-A60A-E7CC1FC652F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0288E0A7-3BF4-44FD-8558-F1571065DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="2910" windowWidth="20880" windowHeight="15705" xr2:uid="{F65BA0A3-315E-4F3B-9DC6-AB09C013BE12}"/>
+    <workbookView xWindow="1215" yWindow="870" windowWidth="21000" windowHeight="19755" xr2:uid="{F65BA0A3-315E-4F3B-9DC6-AB09C013BE12}"/>
   </bookViews>
   <sheets>
     <sheet name="RegQuatTest" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="28">
   <si>
     <t>File name</t>
   </si>
@@ -114,13 +114,16 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>simdQuaternionTests.cpp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,35 +259,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,14 +445,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -586,26 +561,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -651,13 +606,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -703,7 +653,13 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -723,9 +679,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -750,7 +703,7 @@
     <tableColumn id="1" xr3:uid="{3D45B39B-91D3-4BD1-B26D-D142DB4EE292}" name="File name"/>
     <tableColumn id="2" xr3:uid="{15C2718A-8886-4C52-AE07-5523360E72C4}" name=" Function name"/>
     <tableColumn id="3" xr3:uid="{082F66F1-D800-4981-8611-487902182B24}" name=" Time taken"/>
-    <tableColumn id="4" xr3:uid="{50043342-086A-4208-9D48-BC279FE90383}" name="Status" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{50043342-086A-4208-9D48-BC279FE90383}" name="Status" dataDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -765,11 +718,26 @@
     <tableColumn id="1" xr3:uid="{01796C0D-BAC6-4846-A13B-DE4969FD30E5}" name="File name"/>
     <tableColumn id="2" xr3:uid="{26ADFB68-6C10-4CE5-9F13-651D5FA2C2FD}" name=" Function name"/>
     <tableColumn id="3" xr3:uid="{CB9DC4BB-4E98-452D-9FD0-992F68954F55}" name=" Time taken"/>
-    <tableColumn id="4" xr3:uid="{9D4E5634-ACD3-46A6-B5B9-87DD74E423D6}" name="Status" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{9D4E5634-ACD3-46A6-B5B9-87DD74E423D6}" name="Status" dataDxfId="1">
       <calculatedColumnFormula>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AAC3426E-3824-4AF8-9B16-D44C5438302A}" name="Table3" displayName="Table3" ref="E24:H45" totalsRowShown="0">
+  <autoFilter ref="E24:H45" xr:uid="{AAC3426E-3824-4AF8-9B16-D44C5438302A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0FFE80FA-7325-45C8-9B99-E8F00DB6F998}" name="File name"/>
+    <tableColumn id="2" xr3:uid="{2D11CBCC-8CAB-4056-89E6-AB2D7AFC93DA}" name=" Function name"/>
+    <tableColumn id="3" xr3:uid="{77C986BD-DD98-42D0-B754-8E0B778BA7B6}" name=" Time taken"/>
+    <tableColumn id="4" xr3:uid="{60827437-FA34-47F4-AD51-3C1435E5A4E6}" name="Status" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table3[[#This Row],[ Time taken]]&lt;C2,"TRUE","FALSE")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1090,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF22C684-27C7-4C0F-9012-A2764268141B}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:G22"/>
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1071,7 @@
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
   </cols>
@@ -1142,7 +1110,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>195.8</v>
+        <v>197.9</v>
       </c>
       <c r="D2" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1155,7 +1123,7 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <v>168.2</v>
+        <v>172.2</v>
       </c>
       <c r="H2" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1167,7 +1135,7 @@
       </c>
       <c r="K2">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>-27.600000000000023</v>
+        <v>-25.700000000000017</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1178,7 +1146,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>194.7</v>
+        <v>168.5</v>
       </c>
       <c r="D3" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1191,7 +1159,7 @@
         <v>5</v>
       </c>
       <c r="G3">
-        <v>205.7</v>
+        <v>204.7</v>
       </c>
       <c r="H3" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1203,7 +1171,7 @@
       </c>
       <c r="K3">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>11</v>
+        <v>36.199999999999989</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1214,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>337.7</v>
+        <v>341.2</v>
       </c>
       <c r="D4" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1227,7 +1195,7 @@
         <v>6</v>
       </c>
       <c r="G4">
-        <v>425.1</v>
+        <v>394.2</v>
       </c>
       <c r="H4" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1239,7 +1207,7 @@
       </c>
       <c r="K4">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>87.400000000000034</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1250,7 +1218,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>223.6</v>
+        <v>229.3</v>
       </c>
       <c r="D5" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1263,7 +1231,7 @@
         <v>7</v>
       </c>
       <c r="G5">
-        <v>1054.4000000000001</v>
+        <v>1553</v>
       </c>
       <c r="H5" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1275,7 +1243,7 @@
       </c>
       <c r="K5">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>830.80000000000007</v>
+        <v>1323.7</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1286,7 +1254,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>223.7</v>
+        <v>225.7</v>
       </c>
       <c r="D6" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1299,7 +1267,7 @@
         <v>8</v>
       </c>
       <c r="G6">
-        <v>1055</v>
+        <v>1060.5</v>
       </c>
       <c r="H6" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1311,7 +1279,7 @@
       </c>
       <c r="K6">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>831.3</v>
+        <v>834.8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1322,7 +1290,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>597.1</v>
+        <v>596.20000000000005</v>
       </c>
       <c r="D7" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1335,7 +1303,7 @@
         <v>9</v>
       </c>
       <c r="G7">
-        <v>1185.5</v>
+        <v>1182</v>
       </c>
       <c r="H7" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1347,7 +1315,7 @@
       </c>
       <c r="K7">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>588.4</v>
+        <v>585.79999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1358,7 +1326,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>225.9</v>
+        <v>229.9</v>
       </c>
       <c r="D8" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1371,7 +1339,7 @@
         <v>10</v>
       </c>
       <c r="G8">
-        <v>1050.4000000000001</v>
+        <v>1059.3</v>
       </c>
       <c r="H8" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1383,7 +1351,7 @@
       </c>
       <c r="K8">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>824.50000000000011</v>
+        <v>829.4</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1394,7 +1362,7 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>493</v>
+        <v>492.2</v>
       </c>
       <c r="D9" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1407,7 +1375,7 @@
         <v>11</v>
       </c>
       <c r="G9">
-        <v>597.6</v>
+        <v>566.5</v>
       </c>
       <c r="H9" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1419,7 +1387,7 @@
       </c>
       <c r="K9">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>104.60000000000002</v>
+        <v>74.300000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1430,7 +1398,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>524</v>
+        <v>535.1</v>
       </c>
       <c r="D10" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1443,7 +1411,7 @@
         <v>12</v>
       </c>
       <c r="G10">
-        <v>1394.9</v>
+        <v>1406.3</v>
       </c>
       <c r="H10" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1455,7 +1423,7 @@
       </c>
       <c r="K10">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>870.90000000000009</v>
+        <v>871.19999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1466,7 +1434,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>527.29999999999995</v>
+        <v>531.1</v>
       </c>
       <c r="D11" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1479,7 +1447,7 @@
         <v>13</v>
       </c>
       <c r="G11">
-        <v>1402.9</v>
+        <v>1408.5</v>
       </c>
       <c r="H11" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1491,7 +1459,7 @@
       </c>
       <c r="K11">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>875.60000000000014</v>
+        <v>877.4</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1502,7 +1470,7 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>858</v>
+        <v>865.6</v>
       </c>
       <c r="D12" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1515,7 +1483,7 @@
         <v>14</v>
       </c>
       <c r="G12">
-        <v>1720.3</v>
+        <v>1718.1</v>
       </c>
       <c r="H12" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1527,7 +1495,7 @@
       </c>
       <c r="K12">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>862.3</v>
+        <v>852.49999999999989</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1538,7 +1506,7 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>528.79999999999995</v>
+        <v>537.20000000000005</v>
       </c>
       <c r="D13" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1551,7 +1519,7 @@
         <v>15</v>
       </c>
       <c r="G13">
-        <v>581.79999999999995</v>
+        <v>590.20000000000005</v>
       </c>
       <c r="H13" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1574,7 +1542,7 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>186.6</v>
+        <v>183.4</v>
       </c>
       <c r="D14" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1587,7 +1555,7 @@
         <v>16</v>
       </c>
       <c r="G14">
-        <v>699.1</v>
+        <v>742.1</v>
       </c>
       <c r="H14" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1599,7 +1567,7 @@
       </c>
       <c r="K14">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>512.5</v>
+        <v>558.70000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1610,7 +1578,7 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D15" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1623,7 +1591,7 @@
         <v>17</v>
       </c>
       <c r="G15">
-        <v>922.5</v>
+        <v>936.5</v>
       </c>
       <c r="H15" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1635,7 +1603,7 @@
       </c>
       <c r="K15">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>612.5</v>
+        <v>634.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1646,7 +1614,7 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>171.4</v>
+        <v>171.8</v>
       </c>
       <c r="D16" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1659,7 +1627,7 @@
         <v>18</v>
       </c>
       <c r="G16">
-        <v>171.7</v>
+        <v>172.6</v>
       </c>
       <c r="H16" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1671,7 +1639,7 @@
       </c>
       <c r="K16">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>0.29999999999998295</v>
+        <v>0.79999999999998295</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1682,7 +1650,7 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>1593.4</v>
+        <v>1607.5</v>
       </c>
       <c r="D17" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1695,7 +1663,7 @@
         <v>19</v>
       </c>
       <c r="G17">
-        <v>1742.4</v>
+        <v>1751.5</v>
       </c>
       <c r="H17" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1707,7 +1675,7 @@
       </c>
       <c r="K17">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1718,7 +1686,7 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>472.4</v>
+        <v>473.8</v>
       </c>
       <c r="D18" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1731,7 +1699,7 @@
         <v>20</v>
       </c>
       <c r="G18">
-        <v>585</v>
+        <v>567.5</v>
       </c>
       <c r="H18" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1743,7 +1711,7 @@
       </c>
       <c r="K18">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>112.60000000000002</v>
+        <v>93.699999999999989</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1754,7 +1722,7 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>1284.4000000000001</v>
+        <v>1301.5</v>
       </c>
       <c r="D19" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1767,7 +1735,7 @@
         <v>21</v>
       </c>
       <c r="G19">
-        <v>7024.9</v>
+        <v>7048</v>
       </c>
       <c r="H19" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1779,7 +1747,7 @@
       </c>
       <c r="K19">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>5740.5</v>
+        <v>5746.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1790,7 +1758,7 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>991</v>
+        <v>1001.4</v>
       </c>
       <c r="D20" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1803,7 +1771,7 @@
         <v>22</v>
       </c>
       <c r="G20">
-        <v>7070.1</v>
+        <v>7062.7</v>
       </c>
       <c r="H20" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1815,7 +1783,7 @@
       </c>
       <c r="K20">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>6079.1</v>
+        <v>6061.3</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1826,7 +1794,7 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>2385.3000000000002</v>
+        <v>2350.9</v>
       </c>
       <c r="D21" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1839,7 +1807,7 @@
         <v>23</v>
       </c>
       <c r="G21">
-        <v>7020.3</v>
+        <v>7633.8</v>
       </c>
       <c r="H21" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1851,7 +1819,7 @@
       </c>
       <c r="K21">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>4635</v>
+        <v>5282.9</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1862,7 +1830,7 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>1193</v>
+        <v>1209.2</v>
       </c>
       <c r="D22" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1875,7 +1843,7 @@
         <v>24</v>
       </c>
       <c r="G22">
-        <v>2698.8</v>
+        <v>2724.6</v>
       </c>
       <c r="H22" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1887,717 +1855,523 @@
       </c>
       <c r="K22">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>1505.8000000000002</v>
+        <v>1515.3999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" t="str">
+        <f>B2</f>
+        <v>construction(void)</v>
+      </c>
+      <c r="K24">
+        <f>C2-G25</f>
+        <v>3.3000000000000114</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>2</v>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>194.6</v>
+      </c>
+      <c r="H25" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C2,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" ref="J25:J45" si="0">B3</f>
+        <v>copyConstruct(void)</v>
+      </c>
+      <c r="K25">
+        <f t="shared" ref="K25:K44" si="1">C3-G26</f>
+        <v>-18.900000000000006</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="3">
-        <v>195.8</v>
-      </c>
-      <c r="D26" s="5" t="str">
-        <f>IF(C26&lt;G26,"TRUE","FALSE")</f>
-        <v>TRUE</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="3">
-        <v>199</v>
-      </c>
-      <c r="H26" s="5" t="str">
-        <f>IF(G26&lt;C26,"TRUE","FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="J26">
-        <f>G26-C26</f>
-        <v>3.1999999999999886</v>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>187.4</v>
+      </c>
+      <c r="H26" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C3,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>assignment(void)</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>-6.1000000000000227</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4">
-        <v>194.7</v>
-      </c>
-      <c r="D27" s="5" t="str">
-        <f t="shared" ref="D27:D46" si="0">IF(C27&lt;G27,"TRUE","FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" s="4">
-        <v>186</v>
-      </c>
-      <c r="H27" s="5" t="str">
-        <f t="shared" ref="H27:H46" si="1">IF(G27&lt;C27,"TRUE","FALSE")</f>
-        <v>TRUE</v>
-      </c>
-      <c r="J27">
-        <f t="shared" ref="J27:J46" si="2">G27-C27</f>
-        <v>-8.6999999999999886</v>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>347.3</v>
+      </c>
+      <c r="H27" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C4,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>addAssign(void)</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>-1020.8</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="3">
-        <v>337.7</v>
-      </c>
-      <c r="D28" s="5" t="str">
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>1250.0999999999999</v>
+      </c>
+      <c r="H28" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C5,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G28" s="3">
-        <v>340.2</v>
-      </c>
-      <c r="H28" s="5" t="str">
+        <v>subAssign(void)</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>-1036</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="4">
-        <v>223.6</v>
-      </c>
-      <c r="D29" s="5" t="str">
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <v>1261.7</v>
+      </c>
+      <c r="H29" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C6,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="4">
-        <v>224.5</v>
-      </c>
-      <c r="H29" s="5" t="str">
+        <v>mulQuatAssign(void)</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="2"/>
-        <v>0.90000000000000568</v>
+        <v>-2388.3000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="3">
-        <v>223.7</v>
-      </c>
-      <c r="D30" s="5" t="str">
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <v>2984.5</v>
+      </c>
+      <c r="H30" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C7,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="3">
-        <v>226.5</v>
-      </c>
-      <c r="H30" s="5" t="str">
+        <v>mulScaleAssign(void)</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="2"/>
-        <v>2.8000000000000114</v>
+        <v>-703.30000000000007</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="4">
-        <v>597.1</v>
-      </c>
-      <c r="D31" s="5" t="str">
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31">
+        <v>933.2</v>
+      </c>
+      <c r="H31" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C8,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="4">
-        <v>595.4</v>
-      </c>
-      <c r="H31" s="5" t="str">
+        <v>negation(void)</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="2"/>
-        <v>-1.7000000000000455</v>
+        <v>-11.600000000000023</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="3">
-        <v>225.9</v>
-      </c>
-      <c r="D32" s="5" t="str">
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32">
+        <v>503.8</v>
+      </c>
+      <c r="H32" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C9,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="3">
-        <v>226.1</v>
-      </c>
-      <c r="H32" s="5" t="str">
+        <v>add(void)</v>
+      </c>
+      <c r="K32">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="2"/>
-        <v>0.19999999999998863</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="4">
-        <v>493</v>
-      </c>
-      <c r="D33" s="5" t="str">
+        <v>-871.19999999999993</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33">
+        <v>1406.3</v>
+      </c>
+      <c r="H33" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C10,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="4">
-        <v>495</v>
-      </c>
-      <c r="H33" s="5" t="str">
+        <v>sub(void)</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="3">
-        <v>524</v>
-      </c>
-      <c r="D34" s="5" t="str">
+        <v>-807.80000000000007</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34">
+        <v>1338.9</v>
+      </c>
+      <c r="H34" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C11,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="3">
-        <v>529.29999999999995</v>
-      </c>
-      <c r="H34" s="5" t="str">
+        <v>mulQuat(void)</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="2"/>
-        <v>5.2999999999999545</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="4">
-        <v>527.29999999999995</v>
-      </c>
-      <c r="D35" s="5" t="str">
+        <v>-2151.8000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35">
+        <v>3017.4</v>
+      </c>
+      <c r="H35" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C12,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="4">
-        <v>527.70000000000005</v>
-      </c>
-      <c r="H35" s="5" t="str">
+        <v>mulScale(void)</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="2"/>
-        <v>0.40000000000009095</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="3">
-        <v>858</v>
-      </c>
-      <c r="D36" s="5" t="str">
+        <v>-796.7</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36">
+        <v>1333.9</v>
+      </c>
+      <c r="H36" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C13,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="3">
-        <v>865.4</v>
-      </c>
-      <c r="H36" s="5" t="str">
+        <v>dot(void)</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="2"/>
-        <v>7.3999999999999773</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="4">
-        <v>528.79999999999995</v>
-      </c>
-      <c r="D37" s="5" t="str">
+        <v>-1163.1999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37">
+        <v>1346.6</v>
+      </c>
+      <c r="H37" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C14,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J37" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="4">
-        <v>532.4</v>
-      </c>
-      <c r="H37" s="5" t="str">
+        <v>norm(void)</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="2"/>
-        <v>3.6000000000000227</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="3">
-        <v>186.6</v>
-      </c>
-      <c r="D38" s="5" t="str">
+        <v>-1001.4000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38">
+        <v>1303.4000000000001</v>
+      </c>
+      <c r="H38" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C15,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="3">
-        <v>185.7</v>
-      </c>
-      <c r="H38" s="5" t="str">
+        <v>normSquared(void)</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="2"/>
-        <v>-0.90000000000000568</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="4">
-        <v>310</v>
-      </c>
-      <c r="D39" s="5" t="str">
+        <v>-1069.8</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39">
+        <v>1241.5999999999999</v>
+      </c>
+      <c r="H39" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C16,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="4">
-        <v>302.8</v>
-      </c>
-      <c r="H39" s="5" t="str">
+        <v>normalize(void)</v>
+      </c>
+      <c r="K39">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="2"/>
-        <v>-7.1999999999999886</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="3">
-        <v>171.4</v>
-      </c>
-      <c r="D40" s="5" t="str">
+        <v>-1680.1</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40">
+        <v>3287.6</v>
+      </c>
+      <c r="H40" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C17,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="3">
-        <v>173.4</v>
-      </c>
-      <c r="H40" s="5" t="str">
+        <v>conjugate(void)</v>
+      </c>
+      <c r="K40">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1593.4</v>
-      </c>
-      <c r="D41" s="5" t="str">
+        <v>-1.0999999999999659</v>
+      </c>
+    </row>
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41">
+        <v>474.9</v>
+      </c>
+      <c r="H41" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C18,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="4">
-        <v>1609.4</v>
-      </c>
-      <c r="H41" s="5" t="str">
+        <v>rotateVectorFromFloats(void)</v>
+      </c>
+      <c r="K41">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="3">
-        <v>472.4</v>
-      </c>
-      <c r="D42" s="5" t="str">
+        <v>-0.40000000000009095</v>
+      </c>
+    </row>
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42">
+        <v>1301.9000000000001</v>
+      </c>
+      <c r="H42" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C19,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" s="3">
-        <v>476.4</v>
-      </c>
-      <c r="H42" s="5" t="str">
+        <v>rotateVectorFromArray(void)</v>
+      </c>
+      <c r="K42">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="4">
-        <v>1284.4000000000001</v>
-      </c>
-      <c r="D43" s="5" t="str">
+        <v>0.39999999999997726</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43">
+        <v>1001</v>
+      </c>
+      <c r="H43" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C20,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" s="4">
-        <v>1299.9000000000001</v>
-      </c>
-      <c r="H43" s="5" t="str">
+        <v>fromEuler(void)</v>
+      </c>
+      <c r="K43">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="2"/>
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="3">
-        <v>991</v>
-      </c>
-      <c r="D44" s="5" t="str">
+        <v>2.3000000000001819</v>
+      </c>
+    </row>
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44">
+        <v>2348.6</v>
+      </c>
+      <c r="H44" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C21,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="3">
-        <v>1024.2</v>
-      </c>
-      <c r="H44" s="5" t="str">
+        <v>fromAxisAngle(void)</v>
+      </c>
+      <c r="K44">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="2"/>
-        <v>33.200000000000045</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="4">
-        <v>2385.3000000000002</v>
-      </c>
-      <c r="D45" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="4">
-        <v>2364</v>
-      </c>
-      <c r="H45" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>TRUE</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="2"/>
-        <v>-21.300000000000182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="2" t="s">
+        <v>5.6000000000001364</v>
+      </c>
+    </row>
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="2">
-        <v>1193</v>
-      </c>
-      <c r="D46" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="2">
-        <v>1200.3</v>
-      </c>
-      <c r="H46" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="2"/>
-        <v>7.2999999999999545</v>
+      <c r="G45">
+        <v>1203.5999999999999</v>
+      </c>
+      <c r="H45" t="str">
+        <f>IF(Table3[[#This Row],[ Time taken]]&lt;C22,"TRUE","FALSE")</f>
+        <v>TRUE</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="D23:D25 D48:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+  <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="D23 D56:D1048576">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"""FALSE"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1 K2:K22 J23:J1048576">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="J1 K2:K22 J23:J1048576 K24:K44">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved quaternion to be header only.
Added constexpr on many of the quaternion functions.
</commit_message>
<xml_diff>
--- a/build/Visual Studio Community 2022 Release - amd64/Debug/Debug/GLMREGComparison.xlsx
+++ b/build/Visual Studio Community 2022 Release - amd64/Debug/Debug/GLMREGComparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelson\Documents\Projects\typed_squirrel\build\Visual Studio Community 2022 Release - amd64\Debug\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630D796D-3060-4B79-AF68-CC033FB74B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFA871D-404A-47D4-81AB-C326B6113C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="2910" windowWidth="20880" windowHeight="15705" xr2:uid="{F65BA0A3-315E-4F3B-9DC6-AB09C013BE12}"/>
+    <workbookView xWindow="240" yWindow="1980" windowWidth="21000" windowHeight="19755" xr2:uid="{F65BA0A3-315E-4F3B-9DC6-AB09C013BE12}"/>
   </bookViews>
   <sheets>
     <sheet name="RegQuatTest" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="31">
   <si>
     <t>File name</t>
   </si>
@@ -114,13 +114,25 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>quaternionOldTests.cpp</t>
+  </si>
+  <si>
+    <t>Current Quaternion</t>
+  </si>
+  <si>
+    <t>GLM Quaternion</t>
+  </si>
+  <si>
+    <t>Old Quaternion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,35 +268,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,14 +461,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -586,26 +577,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -651,13 +622,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -703,7 +672,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -744,13 +722,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{710BCFAD-6C59-4AA4-9C69-F65EDE7B7130}" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0">
-  <autoFilter ref="A1:D22" xr:uid="{710BCFAD-6C59-4AA4-9C69-F65EDE7B7130}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{710BCFAD-6C59-4AA4-9C69-F65EDE7B7130}" name="Table1" displayName="Table1" ref="A3:D24" totalsRowShown="0">
+  <autoFilter ref="A3:D24" xr:uid="{710BCFAD-6C59-4AA4-9C69-F65EDE7B7130}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3D45B39B-91D3-4BD1-B26D-D142DB4EE292}" name="File name"/>
     <tableColumn id="2" xr3:uid="{15C2718A-8886-4C52-AE07-5523360E72C4}" name=" Function name"/>
     <tableColumn id="3" xr3:uid="{082F66F1-D800-4981-8611-487902182B24}" name=" Time taken"/>
-    <tableColumn id="4" xr3:uid="{50043342-086A-4208-9D48-BC279FE90383}" name="Status" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{50043342-086A-4208-9D48-BC279FE90383}" name="Status" dataDxfId="6">
       <calculatedColumnFormula>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -759,17 +737,53 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45FE94CF-0F34-4DB5-B60F-4A5DD5605B64}" name="Table2" displayName="Table2" ref="E1:H22" totalsRowShown="0">
-  <autoFilter ref="E1:H22" xr:uid="{45FE94CF-0F34-4DB5-B60F-4A5DD5605B64}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45FE94CF-0F34-4DB5-B60F-4A5DD5605B64}" name="Table2" displayName="Table2" ref="E3:H24" totalsRowShown="0">
+  <autoFilter ref="E3:H24" xr:uid="{45FE94CF-0F34-4DB5-B60F-4A5DD5605B64}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{01796C0D-BAC6-4846-A13B-DE4969FD30E5}" name="File name"/>
     <tableColumn id="2" xr3:uid="{26ADFB68-6C10-4CE5-9F13-651D5FA2C2FD}" name=" Function name"/>
     <tableColumn id="3" xr3:uid="{CB9DC4BB-4E98-452D-9FD0-992F68954F55}" name=" Time taken"/>
-    <tableColumn id="4" xr3:uid="{9D4E5634-ACD3-46A6-B5B9-87DD74E423D6}" name="Status" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{9D4E5634-ACD3-46A6-B5B9-87DD74E423D6}" name="Status" dataDxfId="5">
       <calculatedColumnFormula>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F4E14AC9-C9DB-465D-A9B5-25ACBFB65156}" name="Table3" displayName="Table3" ref="E27:H48" totalsRowShown="0">
+  <autoFilter ref="E27:H48" xr:uid="{F4E14AC9-C9DB-465D-A9B5-25ACBFB65156}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{5666163B-F488-464F-8008-5B021B2E2D8D}" name="File name"/>
+    <tableColumn id="2" xr3:uid="{30BAC214-A4D0-403B-AD20-3A837A9CAF54}" name=" Function name"/>
+    <tableColumn id="3" xr3:uid="{CE3682FE-722F-4B02-86AD-CD58AF48952C}" name=" Time taken"/>
+    <tableColumn id="4" xr3:uid="{475C2DC7-3377-4DBD-AC94-CFD7C72C815F}" name="Status">
+      <calculatedColumnFormula>IF(G28&lt;C28,"TRUE","FALSE")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D014F68D-938A-477D-950E-7EED0ACAEDDC}" name="Table5" displayName="Table5" ref="A27:D48" totalsRowShown="0">
+  <autoFilter ref="A27:D48" xr:uid="{D014F68D-938A-477D-950E-7EED0ACAEDDC}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6DE51BE5-BECE-49DF-A4A6-58F1A7C361A5}" name="File name" dataDxfId="2">
+      <calculatedColumnFormula>A4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{DC4E0F68-37DB-4B47-9AC6-B2EDB2495C4E}" name=" Function name" dataDxfId="1">
+      <calculatedColumnFormula>B4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{408DA077-7517-4E94-BF97-3D3732BC1BD7}" name=" Time taken" dataDxfId="0">
+      <calculatedColumnFormula>C4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{581B3196-2027-41A4-B11D-996B626BCD13}" name="Status">
+      <calculatedColumnFormula>IF(C28&lt;G28,"TRUE","FALSE")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1090,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF22C684-27C7-4C0F-9012-A2764268141B}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:G46"/>
+      <selection activeCell="A4" sqref="A4:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,109 +1115,62 @@
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>199</v>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>174.4</v>
-      </c>
-      <c r="H2" t="str">
-        <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
-        <v>TRUE</v>
-      </c>
-      <c r="J2" t="str">
-        <f>Table1[[#This Row],[ Function name]]</f>
-        <v>construction(void)</v>
-      </c>
-      <c r="K2">
-        <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>-24.599999999999994</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>186</v>
-      </c>
-      <c r="D3" t="str">
-        <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
-        <v>TRUE</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>206.5</v>
-      </c>
-      <c r="H3" t="str">
-        <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="J3" t="str">
-        <f>Table1[[#This Row],[ Function name]]</f>
-        <v>copyConstruct(void)</v>
-      </c>
-      <c r="K3">
-        <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>20.5</v>
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1211,35 +1178,35 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>340.2</v>
+        <v>204.7</v>
       </c>
       <c r="D4" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
-        <v>TRUE</v>
+        <v>FALSE</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>394.8</v>
+        <v>183.2</v>
       </c>
       <c r="H4" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J4" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>assignment(void)</v>
+        <v>construction(void)</v>
       </c>
       <c r="K4">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>54.600000000000023</v>
+        <v>-21.5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1247,10 +1214,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>224.5</v>
+        <v>168.5</v>
       </c>
       <c r="D5" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1260,10 +1227,10 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>1058.9000000000001</v>
+        <v>204.1</v>
       </c>
       <c r="H5" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1271,11 +1238,11 @@
       </c>
       <c r="J5" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>addAssign(void)</v>
+        <v>copyConstruct(void)</v>
       </c>
       <c r="K5">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>834.40000000000009</v>
+        <v>35.599999999999994</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1283,10 +1250,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>226.5</v>
+        <v>350</v>
       </c>
       <c r="D6" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1296,10 +1263,10 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6">
-        <v>1063.5999999999999</v>
+        <v>395.5</v>
       </c>
       <c r="H6" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1307,11 +1274,11 @@
       </c>
       <c r="J6" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>subAssign(void)</v>
+        <v>assignment(void)</v>
       </c>
       <c r="K6">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>837.09999999999991</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1319,10 +1286,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>595.4</v>
+        <v>226</v>
       </c>
       <c r="D7" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1332,10 +1299,10 @@
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7">
-        <v>1210.4000000000001</v>
+        <v>1091.9000000000001</v>
       </c>
       <c r="H7" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1343,11 +1310,11 @@
       </c>
       <c r="J7" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>mulQuatAssign(void)</v>
+        <v>addAssign(void)</v>
       </c>
       <c r="K7">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>615.00000000000011</v>
+        <v>865.90000000000009</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1355,10 +1322,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>226.1</v>
+        <v>225.9</v>
       </c>
       <c r="D8" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1368,10 +1335,10 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>1056.0999999999999</v>
+        <v>1081</v>
       </c>
       <c r="H8" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1379,11 +1346,11 @@
       </c>
       <c r="J8" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>mulScaleAssign(void)</v>
+        <v>subAssign(void)</v>
       </c>
       <c r="K8">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>829.99999999999989</v>
+        <v>855.1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1391,10 +1358,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>495</v>
+        <v>601.29999999999995</v>
       </c>
       <c r="D9" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1404,10 +1371,10 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9">
-        <v>601.79999999999995</v>
+        <v>1198.7</v>
       </c>
       <c r="H9" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1415,11 +1382,11 @@
       </c>
       <c r="J9" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>negation(void)</v>
+        <v>mulQuatAssign(void)</v>
       </c>
       <c r="K9">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>106.79999999999995</v>
+        <v>597.40000000000009</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1427,10 +1394,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>529.29999999999995</v>
+        <v>227.3</v>
       </c>
       <c r="D10" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1440,10 +1407,10 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10">
-        <v>1418.9</v>
+        <v>1046.4000000000001</v>
       </c>
       <c r="H10" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1451,11 +1418,11 @@
       </c>
       <c r="J10" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>add(void)</v>
+        <v>mulScaleAssign(void)</v>
       </c>
       <c r="K10">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>889.60000000000014</v>
+        <v>819.10000000000014</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1463,10 +1430,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>527.70000000000005</v>
+        <v>522.9</v>
       </c>
       <c r="D11" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1476,10 +1443,10 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G11">
-        <v>1412.4</v>
+        <v>595.6</v>
       </c>
       <c r="H11" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1487,11 +1454,11 @@
       </c>
       <c r="J11" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>sub(void)</v>
+        <v>negation(void)</v>
       </c>
       <c r="K11">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>884.7</v>
+        <v>72.700000000000045</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1499,10 +1466,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12">
-        <v>865.4</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="D12" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1512,10 +1479,10 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>1724.7</v>
+        <v>1400.7</v>
       </c>
       <c r="H12" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1523,11 +1490,11 @@
       </c>
       <c r="J12" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>mulQuat(void)</v>
+        <v>add(void)</v>
       </c>
       <c r="K12">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>859.30000000000007</v>
+        <v>815</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1535,10 +1502,10 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>532.4</v>
+        <v>614.29999999999995</v>
       </c>
       <c r="D13" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1548,10 +1515,10 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G13">
-        <v>587.1</v>
+        <v>1390.9</v>
       </c>
       <c r="H13" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1559,11 +1526,11 @@
       </c>
       <c r="J13" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>mulScale(void)</v>
+        <v>sub(void)</v>
       </c>
       <c r="K13">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>54.700000000000045</v>
+        <v>776.60000000000014</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1571,10 +1538,10 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>185.7</v>
+        <v>975.6</v>
       </c>
       <c r="D14" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1584,10 +1551,10 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G14">
-        <v>713.4</v>
+        <v>1714.3</v>
       </c>
       <c r="H14" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1595,11 +1562,11 @@
       </c>
       <c r="J14" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>dot(void)</v>
+        <v>mulQuat(void)</v>
       </c>
       <c r="K14">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>527.70000000000005</v>
+        <v>738.69999999999993</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1607,35 +1574,35 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>302.8</v>
+        <v>694</v>
       </c>
       <c r="D15" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
-        <v>TRUE</v>
+        <v>FALSE</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G15">
-        <v>935.6</v>
+        <v>580.29999999999995</v>
       </c>
       <c r="H15" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J15" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>norm(void)</v>
+        <v>mulScale(void)</v>
       </c>
       <c r="K15">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>632.79999999999995</v>
+        <v>-113.70000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1643,10 +1610,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16">
-        <v>173.4</v>
+        <v>219.6</v>
       </c>
       <c r="D16" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1656,10 +1623,10 @@
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G16">
-        <v>173.9</v>
+        <v>694.5</v>
       </c>
       <c r="H16" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1667,11 +1634,11 @@
       </c>
       <c r="J16" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>normSquared(void)</v>
+        <v>dot(void)</v>
       </c>
       <c r="K16">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>0.5</v>
+        <v>474.9</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1679,10 +1646,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17">
-        <v>1609.4</v>
+        <v>370</v>
       </c>
       <c r="D17" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1692,10 +1659,10 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G17">
-        <v>1759.6</v>
+        <v>922.5</v>
       </c>
       <c r="H17" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1703,11 +1670,11 @@
       </c>
       <c r="J17" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>normalize(void)</v>
+        <v>norm(void)</v>
       </c>
       <c r="K17">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>150.19999999999982</v>
+        <v>552.5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1715,35 +1682,35 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18">
-        <v>476.4</v>
+        <v>235.6</v>
       </c>
       <c r="D18" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
-        <v>TRUE</v>
+        <v>FALSE</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G18">
-        <v>592.4</v>
+        <v>171.4</v>
       </c>
       <c r="H18" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J18" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>conjugate(void)</v>
+        <v>normSquared(void)</v>
       </c>
       <c r="K18">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>116</v>
+        <v>-64.199999999999989</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1751,10 +1718,10 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19">
-        <v>1299.9000000000001</v>
+        <v>1445.9</v>
       </c>
       <c r="D19" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1764,10 +1731,10 @@
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G19">
-        <v>7114.3</v>
+        <v>1738.9</v>
       </c>
       <c r="H19" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1775,11 +1742,11 @@
       </c>
       <c r="J19" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>rotateVectorFromFloats(void)</v>
+        <v>normalize(void)</v>
       </c>
       <c r="K19">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>5814.4</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1787,35 +1754,35 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20">
-        <v>1024.2</v>
+        <v>629.79999999999995</v>
       </c>
       <c r="D20" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
-        <v>TRUE</v>
+        <v>FALSE</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G20">
-        <v>7181.3</v>
+        <v>607.9</v>
       </c>
       <c r="H20" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
-        <v>FALSE</v>
+        <v>TRUE</v>
       </c>
       <c r="J20" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>rotateVectorFromArray(void)</v>
+        <v>conjugate(void)</v>
       </c>
       <c r="K20">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>6157.1</v>
+        <v>-21.899999999999977</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1823,10 +1790,10 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21">
-        <v>2364</v>
+        <v>1317.9</v>
       </c>
       <c r="D21" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1836,10 +1803,10 @@
         <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G21">
-        <v>7120.6</v>
+        <v>7011.9</v>
       </c>
       <c r="H21" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1847,11 +1814,11 @@
       </c>
       <c r="J21" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>fromEuler(void)</v>
+        <v>rotateVectorFromFloats(void)</v>
       </c>
       <c r="K21">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>4756.6000000000004</v>
+        <v>5694</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1859,10 +1826,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22">
-        <v>1200.3</v>
+        <v>1014.5</v>
       </c>
       <c r="D22" t="str">
         <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
@@ -1872,10 +1839,10 @@
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G22">
-        <v>2726.3</v>
+        <v>7111.2</v>
       </c>
       <c r="H22" t="str">
         <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
@@ -1883,721 +1850,979 @@
       </c>
       <c r="J22" t="str">
         <f>Table1[[#This Row],[ Function name]]</f>
-        <v>fromAxisAngle(void)</v>
+        <v>rotateVectorFromArray(void)</v>
       </c>
       <c r="K22">
         <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
-        <v>1526.0000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>6096.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23">
+        <v>1858.1</v>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23">
+        <v>7006.3</v>
+      </c>
+      <c r="H23" t="str">
+        <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J23" t="str">
+        <f>Table1[[#This Row],[ Function name]]</f>
+        <v>fromEuler(void)</v>
+      </c>
+      <c r="K23">
+        <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
+        <v>5148.2000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>1231.0999999999999</v>
+      </c>
+      <c r="D24" t="str">
+        <f>IF(Table1[[#This Row],[ Time taken]]&lt;Table2[[#This Row],[ Time taken]], "TRUE", "FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24">
+        <v>2714.6</v>
+      </c>
+      <c r="H24" t="str">
+        <f>IF(Table2[[#This Row],[ Time taken]]&lt;Table1[[#This Row],[ Time taken]],"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J24" t="str">
+        <f>Table1[[#This Row],[ Function name]]</f>
+        <v>fromAxisAngle(void)</v>
+      </c>
+      <c r="K24">
+        <f>Table2[[#This Row],[ Time taken]]-Table1[[#This Row],[ Time taken]]</f>
+        <v>1483.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C27" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F27" t="s">
         <v>1</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G27" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" ref="A28:C48" si="0">A4</f>
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" ref="B28:B48" si="1">B4</f>
+        <v>construction(void)</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:C48" si="2">C4</f>
+        <v>204.7</v>
+      </c>
+      <c r="D28" t="str">
+        <f>IF(C28&lt;G28,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="3">
-        <v>199</v>
-      </c>
-      <c r="D26" s="5" t="str">
-        <f>IF(C26&lt;G26,"TRUE","FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="3">
-        <v>199</v>
-      </c>
-      <c r="H26" s="5" t="str">
-        <f>IF(G26&lt;C26,"TRUE","FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="J26">
-        <f>G26-C26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="G28">
+        <v>211.9</v>
+      </c>
+      <c r="H28" t="str">
+        <f>IF(G28&lt;C28,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J28" t="str">
+        <f>Table5[[#This Row],[ Function name]]</f>
+        <v>construction(void)</v>
+      </c>
+      <c r="K28">
+        <f>G28-C28</f>
+        <v>7.2000000000000171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="1"/>
+        <v>copyConstruct(void)</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>168.5</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" ref="D29:D48" si="3">IF(C29&lt;G29,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="4">
-        <v>186</v>
-      </c>
-      <c r="D27" s="5" t="str">
-        <f t="shared" ref="D27:D46" si="0">IF(C27&lt;G27,"TRUE","FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" s="4">
-        <v>186</v>
-      </c>
-      <c r="H27" s="5" t="str">
-        <f t="shared" ref="H27:H46" si="1">IF(G27&lt;C27,"TRUE","FALSE")</f>
-        <v>FALSE</v>
-      </c>
-      <c r="J27">
-        <f t="shared" ref="J27:J46" si="2">G27-C27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="G29">
+        <v>194.1</v>
+      </c>
+      <c r="H29" t="str">
+        <f>IF(G29&lt;C29,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J29" t="str">
+        <f>B29</f>
+        <v>copyConstruct(void)</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ref="K29:K48" si="4">G29-C29</f>
+        <v>25.599999999999994</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="1"/>
+        <v>assignment(void)</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>350</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="3">
-        <v>340.2</v>
-      </c>
-      <c r="D28" s="5" t="str">
+      <c r="G30">
+        <v>339.6</v>
+      </c>
+      <c r="H30" t="str">
+        <f>IF(G30&lt;C30,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" ref="J30:J48" si="5">B30</f>
+        <v>assignment(void)</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="4"/>
+        <v>-10.399999999999977</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G28" s="3">
-        <v>340.2</v>
-      </c>
-      <c r="H28" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B31" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J28">
+        <v>addAssign(void)</v>
+      </c>
+      <c r="C31">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="4">
-        <v>224.5</v>
-      </c>
-      <c r="D29" s="5" t="str">
+      <c r="G31">
+        <v>225.6</v>
+      </c>
+      <c r="H31" t="str">
+        <f>IF(G31&lt;C31,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="5"/>
+        <v>addAssign(void)</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="4"/>
+        <v>-0.40000000000000568</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="4">
-        <v>224.5</v>
-      </c>
-      <c r="H29" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B32" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J29">
+        <v>subAssign(void)</v>
+      </c>
+      <c r="C32">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="3" t="s">
+        <v>225.9</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="3">
-        <v>226.5</v>
-      </c>
-      <c r="D30" s="5" t="str">
+      <c r="G32">
+        <v>225.2</v>
+      </c>
+      <c r="H32" t="str">
+        <f>IF(G32&lt;C32,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="5"/>
+        <v>subAssign(void)</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="4"/>
+        <v>-0.70000000000001705</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="3">
-        <v>226.5</v>
-      </c>
-      <c r="H30" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B33" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J30">
+        <v>mulQuatAssign(void)</v>
+      </c>
+      <c r="C33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="4" t="s">
+        <v>601.29999999999995</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="3"/>
+        <v>TRUE</v>
+      </c>
+      <c r="E33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="4">
-        <v>595.4</v>
-      </c>
-      <c r="D31" s="5" t="str">
+      <c r="G33">
+        <v>613.1</v>
+      </c>
+      <c r="H33" t="str">
+        <f>IF(G33&lt;C33,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="5"/>
+        <v>mulQuatAssign(void)</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="4"/>
+        <v>11.800000000000068</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="4">
-        <v>595.4</v>
-      </c>
-      <c r="H31" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B34" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J31">
+        <v>mulScaleAssign(void)</v>
+      </c>
+      <c r="C34">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="3" t="s">
+        <v>227.3</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="3"/>
+        <v>TRUE</v>
+      </c>
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="3">
-        <v>226.1</v>
-      </c>
-      <c r="D32" s="5" t="str">
+      <c r="G34">
+        <v>229.9</v>
+      </c>
+      <c r="H34" t="str">
+        <f>IF(G34&lt;C34,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="5"/>
+        <v>mulScaleAssign(void)</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="4"/>
+        <v>2.5999999999999943</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="3">
-        <v>226.1</v>
-      </c>
-      <c r="H32" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B35" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J32">
+        <v>negation(void)</v>
+      </c>
+      <c r="C35">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="4" t="s">
+        <v>522.9</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="3"/>
+        <v>TRUE</v>
+      </c>
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="4">
-        <v>495</v>
-      </c>
-      <c r="D33" s="5" t="str">
+      <c r="G35">
+        <v>595.20000000000005</v>
+      </c>
+      <c r="H35" t="str">
+        <f>IF(G35&lt;C35,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="5"/>
+        <v>negation(void)</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="4"/>
+        <v>72.300000000000068</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="4">
-        <v>495</v>
-      </c>
-      <c r="H33" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B36" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J33">
+        <v>add(void)</v>
+      </c>
+      <c r="C36">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="3" t="s">
+        <v>585.70000000000005</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="3"/>
+        <v>TRUE</v>
+      </c>
+      <c r="E36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="3">
-        <v>529.29999999999995</v>
-      </c>
-      <c r="D34" s="5" t="str">
+      <c r="G36">
+        <v>594.1</v>
+      </c>
+      <c r="H36" t="str">
+        <f>IF(G36&lt;C36,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="5"/>
+        <v>add(void)</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="4"/>
+        <v>8.3999999999999773</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="3">
-        <v>529.29999999999995</v>
-      </c>
-      <c r="H34" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B37" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J34">
+        <v>sub(void)</v>
+      </c>
+      <c r="C37">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="4" t="s">
+        <v>614.29999999999995</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E37" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="4">
-        <v>527.70000000000005</v>
-      </c>
-      <c r="D35" s="5" t="str">
+      <c r="G37">
+        <v>538.4</v>
+      </c>
+      <c r="H37" t="str">
+        <f>IF(G37&lt;C37,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="5"/>
+        <v>sub(void)</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="4"/>
+        <v>-75.899999999999977</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="4">
-        <v>527.70000000000005</v>
-      </c>
-      <c r="H35" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B38" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J35">
+        <v>mulQuat(void)</v>
+      </c>
+      <c r="C38">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="3" t="s">
+        <v>975.6</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="3"/>
+        <v>TRUE</v>
+      </c>
+      <c r="E38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="3">
-        <v>865.4</v>
-      </c>
-      <c r="D36" s="5" t="str">
+      <c r="G38">
+        <v>1016.2</v>
+      </c>
+      <c r="H38" t="str">
+        <f>IF(G38&lt;C38,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="5"/>
+        <v>mulQuat(void)</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="4"/>
+        <v>40.600000000000023</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="3">
-        <v>865.4</v>
-      </c>
-      <c r="H36" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B39" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J36">
+        <v>mulScale(void)</v>
+      </c>
+      <c r="C39">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="4">
-        <v>532.4</v>
-      </c>
-      <c r="D37" s="5" t="str">
+      <c r="G39">
+        <v>556.70000000000005</v>
+      </c>
+      <c r="H39" t="str">
+        <f>IF(G39&lt;C39,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="5"/>
+        <v>mulScale(void)</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="4"/>
+        <v>-137.29999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="4">
-        <v>532.4</v>
-      </c>
-      <c r="H37" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B40" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J37">
+        <v>dot(void)</v>
+      </c>
+      <c r="C40">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="3" t="s">
+        <v>219.6</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="3">
-        <v>185.7</v>
-      </c>
-      <c r="D38" s="5" t="str">
+      <c r="G40">
+        <v>183.3</v>
+      </c>
+      <c r="H40" t="str">
+        <f>IF(G40&lt;C40,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="5"/>
+        <v>dot(void)</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="4"/>
+        <v>-36.299999999999983</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="3">
-        <v>185.7</v>
-      </c>
-      <c r="H38" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B41" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J38">
+        <v>norm(void)</v>
+      </c>
+      <c r="C41">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="4">
-        <v>302.8</v>
-      </c>
-      <c r="D39" s="5" t="str">
+      <c r="G41">
+        <v>308</v>
+      </c>
+      <c r="H41" t="str">
+        <f>IF(G41&lt;C41,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="5"/>
+        <v>norm(void)</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="4"/>
+        <v>-62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="4">
-        <v>302.8</v>
-      </c>
-      <c r="H39" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B42" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J39">
+        <v>normSquared(void)</v>
+      </c>
+      <c r="C42">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="3" t="s">
+        <v>235.6</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="3">
-        <v>173.4</v>
-      </c>
-      <c r="D40" s="5" t="str">
+      <c r="G42">
+        <v>172.2</v>
+      </c>
+      <c r="H42" t="str">
+        <f>IF(G42&lt;C42,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="5"/>
+        <v>normSquared(void)</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="4"/>
+        <v>-63.400000000000006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="3">
-        <v>173.4</v>
-      </c>
-      <c r="H40" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B43" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J40">
+        <v>normalize(void)</v>
+      </c>
+      <c r="C43">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="4" t="s">
+        <v>1445.9</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="3"/>
+        <v>TRUE</v>
+      </c>
+      <c r="E43" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="4">
-        <v>1609.4</v>
-      </c>
-      <c r="D41" s="5" t="str">
+      <c r="G43">
+        <v>1607.1</v>
+      </c>
+      <c r="H43" t="str">
+        <f>IF(G43&lt;C43,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="5"/>
+        <v>normalize(void)</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="4"/>
+        <v>161.19999999999982</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="4">
-        <v>1609.4</v>
-      </c>
-      <c r="H41" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B44" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J41">
+        <v>conjugate(void)</v>
+      </c>
+      <c r="C44">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" s="3" t="s">
+        <v>629.79999999999995</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="3">
-        <v>476.4</v>
-      </c>
-      <c r="D42" s="5" t="str">
+      <c r="G44">
+        <v>471.7</v>
+      </c>
+      <c r="H44" t="str">
+        <f>IF(G44&lt;C44,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="5"/>
+        <v>conjugate(void)</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="4"/>
+        <v>-158.09999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" s="3">
-        <v>476.4</v>
-      </c>
-      <c r="H42" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B45" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J42">
+        <v>rotateVectorFromFloats(void)</v>
+      </c>
+      <c r="C45">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="4" t="s">
+        <v>1317.9</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="4">
-        <v>1299.9000000000001</v>
-      </c>
-      <c r="D43" s="5" t="str">
+      <c r="G45">
+        <v>1309.7</v>
+      </c>
+      <c r="H45" t="str">
+        <f>IF(G45&lt;C45,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="5"/>
+        <v>rotateVectorFromFloats(void)</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="4"/>
+        <v>-8.2000000000000455</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" s="4">
-        <v>1299.9000000000001</v>
-      </c>
-      <c r="H43" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B46" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J43">
+        <v>rotateVectorFromArray(void)</v>
+      </c>
+      <c r="C46">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="3" t="s">
+        <v>1014.5</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="3">
-        <v>1024.2</v>
-      </c>
-      <c r="D44" s="5" t="str">
+      <c r="G46">
+        <v>1002</v>
+      </c>
+      <c r="H46" t="str">
+        <f>IF(G46&lt;C46,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="5"/>
+        <v>rotateVectorFromArray(void)</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="4"/>
+        <v>-12.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="3">
-        <v>1024.2</v>
-      </c>
-      <c r="H44" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B47" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J44">
+        <v>fromEuler(void)</v>
+      </c>
+      <c r="C47">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" s="4" t="s">
+        <v>1858.1</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="3"/>
+        <v>TRUE</v>
+      </c>
+      <c r="E47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="4">
-        <v>2364</v>
-      </c>
-      <c r="D45" s="5" t="str">
+      <c r="G47">
+        <v>2316.6999999999998</v>
+      </c>
+      <c r="H47" t="str">
+        <f>IF(G47&lt;C47,"TRUE","FALSE")</f>
+        <v>FALSE</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="5"/>
+        <v>fromEuler(void)</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="4"/>
+        <v>458.59999999999991</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
         <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="4">
-        <v>2364</v>
-      </c>
-      <c r="H45" s="5" t="str">
+        <v>quaternionTests.cpp</v>
+      </c>
+      <c r="B48" t="str">
         <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J45">
+        <v>fromAxisAngle(void)</v>
+      </c>
+      <c r="C48">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="2" t="s">
+        <v>1231.0999999999999</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="3"/>
+        <v>FALSE</v>
+      </c>
+      <c r="E48" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="2">
-        <v>1200.3</v>
-      </c>
-      <c r="D46" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="2">
-        <v>1200.3</v>
-      </c>
-      <c r="H46" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>FALSE</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="G48">
+        <v>1200.5999999999999</v>
+      </c>
+      <c r="H48" t="str">
+        <f>IF(G48&lt;C48,"TRUE","FALSE")</f>
+        <v>TRUE</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="5"/>
+        <v>fromAxisAngle(void)</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="4"/>
+        <v>-30.5</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="D23:D25 D48:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+  <mergeCells count="4">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="A25:D26"/>
+    <mergeCell ref="E25:H26"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="D50:D1048576">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"""FALSE"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1 K2:K22 J23:J1048576">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="J3 K4:K24 J25:J26 J49:J1048576 K27:K48">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>